<commit_message>
12.1 basic json generating
</commit_message>
<xml_diff>
--- a/example/test.xlsx
+++ b/example/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MachineLearning\JSONGenerator\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51CFEA9-CD3E-45A5-85A1-E24D71DEF025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E0FA01-0A2E-427C-91E3-65579748408C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36480" yWindow="-4125" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,7 +526,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="L14" sqref="K14:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="3">
-        <v>13</v>
+        <v>13.25</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>19</v>

</xml_diff>